<commit_message>
regression code and files fix for staging
</commit_message>
<xml_diff>
--- a/data/BppTrend/Updated_Trend_Calculator_For_ReCalculation/2022_Trend_Factors_Calculator.xlsx
+++ b/data/BppTrend/Updated_Trend_Calculator_For_ReCalculation/2022_Trend_Factors_Calculator.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\DDeepika\IdeaProjects\BPPRetroFit\qa_automation\data\BppTrend\Updated_Trend_Calculator_For_ReCalculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\DDeepika\Desktop\BPP_2022\Updated_Trend_Calculator_For_ReCalculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009A3D51-6C62-48E5-9EDD-DE3937D74DE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14415" tabRatio="920" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9825" tabRatio="920" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trends Settings " sheetId="21" r:id="rId1"/>
@@ -19,31 +20,34 @@
     <sheet name="Construction Composite" sheetId="24" r:id="rId5"/>
     <sheet name="Ag Mobile Equip Composite" sheetId="23" r:id="rId6"/>
     <sheet name="Construction Mobile Composite" sheetId="16" r:id="rId7"/>
-    <sheet name="2019 CPI" sheetId="12" r:id="rId8"/>
-    <sheet name="2019 Equip Index Factors" sheetId="3" r:id="rId9"/>
+    <sheet name="2022 CPI" sheetId="12" r:id="rId8"/>
+    <sheet name="2022 Equip Index Factors" sheetId="3" r:id="rId9"/>
     <sheet name="M&amp;E Property Good Factor" sheetId="6" r:id="rId10"/>
-    <sheet name="2019 Agricultural % Good" sheetId="4" r:id="rId11"/>
-    <sheet name="2019 Construction % Good" sheetId="5" r:id="rId12"/>
+    <sheet name="2022 Agricultural % Good" sheetId="4" r:id="rId11"/>
+    <sheet name="2022 Construction % Good" sheetId="5" r:id="rId12"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="CalcTable">[1]ValueTable!$A$5:$AC$50</definedName>
-    <definedName name="Factor_to_Year">'2019 CPI'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'2019 Agricultural % Good'!$A$1:$I$23</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="11">'2019 Construction % Good'!$A$1:$H$23</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'2019 CPI'!$A$1:$D$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'2019 Equip Index Factors'!$A$1:$F$42</definedName>
+    <definedName name="Factor_to_Year">'2022 CPI'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'2022 Agricultural % Good'!$A$1:$I$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">'2022 Construction % Good'!$A$1:$H$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'2022 CPI'!$A$1:$D$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'2022 Equip Index Factors'!$A$1:$F$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Construction Mobile Composite'!$A$1:$E$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'M&amp;E Property Good Factor'!$A$1:$W$42</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -346,14 +350,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="##"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +453,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -886,15 +896,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Comma 2" xfId="4"/>
-    <cellStyle name="Comma 3" xfId="8"/>
+    <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 3 2" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Percent 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Percent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1009,6 +1019,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1044,6 +1071,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1219,7 +1263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1278,14 +1322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A42"/>
     </sheetView>
   </sheetViews>
@@ -3714,13 +3758,13 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A2:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A43"/>
     </sheetView>
   </sheetViews>
@@ -4809,14 +4853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5488,7 +5532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -8416,11 +8460,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -11352,7 +11397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -11950,13 +11995,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
@@ -12423,13 +12468,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E41"/>
     </sheetView>
   </sheetViews>
@@ -13393,13 +13438,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
@@ -13990,15 +14035,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15179,7 +15224,7 @@
         <v>1.00753</v>
       </c>
       <c r="D32" s="45">
-        <f>TRUNC(IF(C32,(D33*C32),""),5)</f>
+        <f t="shared" si="0"/>
         <v>1.19204</v>
       </c>
     </row>
@@ -15254,7 +15299,7 @@
         <v>1.01525</v>
       </c>
       <c r="D37" s="45">
-        <f>TRUNC(IF(C37,(D38*C37),""),5)</f>
+        <f t="shared" si="0"/>
         <v>1.10991</v>
       </c>
     </row>
@@ -15284,7 +15329,7 @@
         <v>1.02</v>
       </c>
       <c r="D39" s="45">
-        <f>TRUNC(IF(C39,(D40*C39),"0"),5)</f>
+        <f t="shared" si="0"/>
         <v>1.0718099999999999</v>
       </c>
     </row>
@@ -15314,7 +15359,7 @@
         <v>1.01</v>
       </c>
       <c r="D41" s="45">
-        <f t="shared" ref="D41" si="1">TRUNC(IF(C41,(D42*C41),"0"),5)</f>
+        <f t="shared" si="0"/>
         <v>1.0302</v>
       </c>
     </row>
@@ -15348,6 +15393,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1" right="0" top="1" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15359,13 +15405,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A2:Q60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A42"/>
     </sheetView>
   </sheetViews>

</xml_diff>